<commit_message>
sen ana 300 with human intervention as xiao suggested
</commit_message>
<xml_diff>
--- a/probiotic/other_models/model_comparison.xlsx
+++ b/probiotic/other_models/model_comparison.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BE75B9-4D6D-431D-AFDD-1D8187091F64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EC5C81-BB9D-4029-A38C-4959BD50FB32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,11 +178,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="178" formatCode="0.000_ "/>
     <numFmt numFmtId="179" formatCode="0.00000_ "/>
+    <numFmt numFmtId="180" formatCode="0_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -226,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -253,6 +254,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -538,7 +542,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -586,7 +590,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="10">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -613,7 +617,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" s="7" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -642,7 +646,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -675,7 +679,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -705,7 +709,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -735,7 +739,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="10">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -765,7 +769,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="10">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -795,7 +799,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="10">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -825,7 +829,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="10">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -856,7 +860,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -886,7 +890,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="10">
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -916,7 +920,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="10">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -949,7 +953,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="10">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">

</xml_diff>